<commit_message>
Checkpoint. Phone styles are better.
</commit_message>
<xml_diff>
--- a/topics.xlsx
+++ b/topics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Topic</t>
   </si>
@@ -34,6 +34,51 @@
   </si>
   <si>
     <t>LectureVsLab</t>
+  </si>
+  <si>
+    <t>course mechanics</t>
+  </si>
+  <si>
+    <t>statistical learning theory framework</t>
+  </si>
+  <si>
+    <t>lecture</t>
+  </si>
+  <si>
+    <t>gradient and stochastic gradient descent</t>
+  </si>
+  <si>
+    <t>convexity</t>
+  </si>
+  <si>
+    <t>excess risk decomposition</t>
+  </si>
+  <si>
+    <t>L1/L2 regularization</t>
+  </si>
+  <si>
+    <t>loss functions</t>
+  </si>
+  <si>
+    <t>optimization methods for Lasso</t>
+  </si>
+  <si>
+    <t>matrix differentiation</t>
+  </si>
+  <si>
+    <t>lab</t>
+  </si>
+  <si>
+    <t>&lt;a href="refs/matrixCookbook-15Nov2012.pdf"&gt;The Matrix Cookbook&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="refs/stanfordCS229-linalg.pdf"&gt;Linear Algebra review&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="refs/bottou-sgd-tricks-2012.pdf&gt;Bottou's SGD Tricks&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>BV Preface, Ch 1</t>
   </si>
 </sst>
 </file>
@@ -402,18 +447,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="38.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="4" max="4" width="113.1640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -432,6 +477,117 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Content from David, tweaks from Domenic
</commit_message>
<xml_diff>
--- a/topics.xlsx
+++ b/topics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="2580" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,10 +75,10 @@
     <t>&lt;a href="refs/stanfordCS229-linalg.pdf"&gt;Linear Algebra review&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href="refs/bottou-sgd-tricks-2012.pdf&gt;Bottou's SGD Tricks&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>BV Preface, Ch 1</t>
+  </si>
+  <si>
+    <t>&lt;a href="refs/bottou-sgd-tricks-2012.pdf&gt;Bottou's SGD Tricks"&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -512,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Added software section and added a bunch of topics.
</commit_message>
<xml_diff>
--- a/topics.xlsx
+++ b/topics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="5020" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>Topic</t>
   </si>
@@ -79,16 +79,126 @@
   </si>
   <si>
     <t>&lt;a href="refs/bottou-sgd-tricks-2012.pdf&gt;Bottou's SGD Tricks"&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>EABV Sec 1-4</t>
+  </si>
+  <si>
+    <t>SVM (cont)</t>
+  </si>
+  <si>
+    <t>kernel methods</t>
+  </si>
+  <si>
+    <t>subgradient descent</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://web.stanford.edu/class/ee364b/lectures.html"&gt;Boyd subgradient notes&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>ensemble methods</t>
+  </si>
+  <si>
+    <t>exponential families</t>
+  </si>
+  <si>
+    <t>generalized linear models</t>
+  </si>
+  <si>
+    <t>Bayesian networks</t>
+  </si>
+  <si>
+    <t>EM algorithm</t>
+  </si>
+  <si>
+    <t>Gaussian mixture models</t>
+  </si>
+  <si>
+    <t>neural networks</t>
+  </si>
+  <si>
+    <t>midterm review</t>
+  </si>
+  <si>
+    <t>Midterm Exam</t>
+  </si>
+  <si>
+    <t>structured prediction</t>
+  </si>
+  <si>
+    <t>HMM</t>
+  </si>
+  <si>
+    <t>Viterbi decoding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lecture </t>
+  </si>
+  <si>
+    <t>Bayesian methods</t>
+  </si>
+  <si>
+    <t>hierarchical models</t>
+  </si>
+  <si>
+    <t>Gibbs sampling</t>
+  </si>
+  <si>
+    <t>Bayesian model selection</t>
+  </si>
+  <si>
+    <t>dimensionality reduction</t>
+  </si>
+  <si>
+    <t>PCA</t>
+  </si>
+  <si>
+    <t>factor analysis</t>
+  </si>
+  <si>
+    <t>catchup and/or advanced topics</t>
+  </si>
+  <si>
+    <t>SlidesNotes</t>
+  </si>
+  <si>
+    <t>Should we make lists in each section separated by ":" or "~"?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,13 +221,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,151 +570,428 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" customWidth="1"/>
-    <col min="4" max="4" width="113.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added in Brian's iPython notebooks and edited the topics some more.
</commit_message>
<xml_diff>
--- a/topics.xlsx
+++ b/topics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Topic</t>
   </si>
@@ -159,13 +159,22 @@
     <t>factor analysis</t>
   </si>
   <si>
-    <t>catchup and/or advanced topics</t>
-  </si>
-  <si>
     <t>SlidesNotes</t>
   </si>
   <si>
     <t>Should we make lists in each section separated by ":" or "~"?</t>
+  </si>
+  <si>
+    <t>bandit problems</t>
+  </si>
+  <si>
+    <t>Thompson sampling</t>
+  </si>
+  <si>
+    <t>UCB strategy</t>
+  </si>
+  <si>
+    <t>catch up and/or advanced topics</t>
   </si>
 </sst>
 </file>
@@ -570,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -602,10 +611,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -947,45 +956,78 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C31">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C32">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C33">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C34">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated lectures.yml and topics.xlsx.
</commit_message>
<xml_diff>
--- a/topics.xlsx
+++ b/topics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11320" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="16440" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
   <si>
     <t>Topic</t>
   </si>
@@ -169,6 +169,57 @@
   </si>
   <si>
     <t>catch up and/or advanced topics</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2015-01-28</t>
+  </si>
+  <si>
+    <t>2015-02-05</t>
+  </si>
+  <si>
+    <t>2015-01-29</t>
+  </si>
+  <si>
+    <t>2015-02-11</t>
+  </si>
+  <si>
+    <t>2015-02-04</t>
+  </si>
+  <si>
+    <t>2015-02-18</t>
+  </si>
+  <si>
+    <t>2015-02-25</t>
+  </si>
+  <si>
+    <t>2015-03-04</t>
+  </si>
+  <si>
+    <t>2015-03-11</t>
+  </si>
+  <si>
+    <t>2015-03-18</t>
+  </si>
+  <si>
+    <t>2015-03-25</t>
+  </si>
+  <si>
+    <t>2015-04-01</t>
+  </si>
+  <si>
+    <t>2015-04-08</t>
+  </si>
+  <si>
+    <t>2015-04-15</t>
+  </si>
+  <si>
+    <t>2015-04-22</t>
+  </si>
+  <si>
+    <t>2015-04-29</t>
   </si>
 </sst>
 </file>
@@ -224,7 +275,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -232,18 +283,59 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,449 +665,561 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="6" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="33.1640625" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="6" max="6" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="B19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="B20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23">
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30">
+      <c r="B30" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32">
+      <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33">
+      <c r="B33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35">
+      <c r="B35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36">
+      <c r="B36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37">
+      <c r="B37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37">
         <v>14</v>
       </c>
     </row>

</xml_diff>